<commit_message>
Added Open Document Formats to allowed list: .odt, .odp, .ods, .odg
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_xlsx.xlsx
+++ b/spec/fixtures/test_xlsx.xlsx
@@ -1,6 +1,98 @@
 
-<file path=theme/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iceraluk/Projects/ccs-conclave-document-get/spec/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B13F9C05-51CA-3341-A6F6-6468A1167C0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1" uniqueCount="1">
+  <si>
+    <t>Iulia was here :)</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -153,25 +245,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -179,25 +271,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -210,21 +302,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -238,7 +330,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -250,32 +342,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -286,9 +378,30 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
-<file path=theme/theme/themeManager.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeManager xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>